<commit_message>
Update Vision example notebook
Signed-off-by: Bram Stoeller <bram.stoeller@alliander.com>
</commit_message>
<xml_diff>
--- a/docs/examples/data/vision/example.xlsx
+++ b/docs/examples/data/vision/example.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25629"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repos\power-grid-model-io\docs\examples\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AL22994\Workspace\power-grid-model-io\docs\examples\data\vision\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D558D487-A463-4B5B-BB6A-9DD07CC06EC5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44F911DC-937D-4164-92EF-B6B999C82C9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Nodes" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="130">
   <si>
     <t>Number</t>
   </si>
@@ -146,15 +146,6 @@
     <t>1</t>
   </si>
   <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
     <t>Cable.Number</t>
   </si>
   <si>
@@ -411,13 +402,25 @@
   </si>
   <si>
     <t>0.0000);0.0000);1.0000</t>
+  </si>
+  <si>
+    <t>First Node</t>
+  </si>
+  <si>
+    <t>Second Node</t>
+  </si>
+  <si>
+    <t>Third Node</t>
+  </si>
+  <si>
+    <t>Fourth Node</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -437,6 +440,12 @@
       <i/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -462,7 +471,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -472,9 +481,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Standaard" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -490,7 +500,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Kantoorthema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -792,41 +802,41 @@
       <pane xSplit="5" ySplit="2" topLeftCell="F3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="I2" sqref="I2"/>
+      <selection pane="bottomRight" activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.5546875" customWidth="1"/>
-    <col min="3" max="3" width="12.109375" customWidth="1"/>
-    <col min="4" max="4" width="5.88671875" customWidth="1"/>
-    <col min="5" max="5" width="6.6640625" customWidth="1"/>
-    <col min="6" max="6" width="13.21875" customWidth="1"/>
-    <col min="7" max="7" width="15.109375" customWidth="1"/>
-    <col min="8" max="8" width="9.21875" customWidth="1"/>
-    <col min="9" max="9" width="14.77734375" customWidth="1"/>
-    <col min="10" max="11" width="5.88671875" customWidth="1"/>
-    <col min="12" max="12" width="17.88671875" customWidth="1"/>
-    <col min="13" max="13" width="16.21875" customWidth="1"/>
-    <col min="14" max="14" width="24.21875" customWidth="1"/>
-    <col min="15" max="15" width="22.88671875" customWidth="1"/>
-    <col min="16" max="16" width="23.5546875" customWidth="1"/>
-    <col min="17" max="17" width="26.44140625" customWidth="1"/>
-    <col min="18" max="18" width="9.33203125" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" customWidth="1"/>
+    <col min="4" max="4" width="5.85546875" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" customWidth="1"/>
+    <col min="6" max="6" width="13.28515625" customWidth="1"/>
+    <col min="7" max="7" width="15.140625" customWidth="1"/>
+    <col min="8" max="8" width="9.28515625" customWidth="1"/>
+    <col min="9" max="9" width="14.7109375" customWidth="1"/>
+    <col min="10" max="11" width="5.85546875" customWidth="1"/>
+    <col min="12" max="12" width="17.85546875" customWidth="1"/>
+    <col min="13" max="13" width="16.28515625" customWidth="1"/>
+    <col min="14" max="14" width="24.28515625" customWidth="1"/>
+    <col min="15" max="15" width="22.85546875" customWidth="1"/>
+    <col min="16" max="16" width="23.5703125" customWidth="1"/>
+    <col min="17" max="17" width="26.42578125" customWidth="1"/>
+    <col min="18" max="18" width="9.28515625" customWidth="1"/>
     <col min="19" max="19" width="16" customWidth="1"/>
-    <col min="20" max="20" width="5.88671875" customWidth="1"/>
-    <col min="21" max="21" width="11.44140625" customWidth="1"/>
-    <col min="22" max="22" width="10.88671875" customWidth="1"/>
-    <col min="23" max="23" width="9.88671875" customWidth="1"/>
-    <col min="24" max="24" width="13.77734375" customWidth="1"/>
-    <col min="25" max="25" width="11.109375" customWidth="1"/>
-    <col min="26" max="26" width="8.77734375" customWidth="1"/>
-    <col min="27" max="28" width="5.88671875" customWidth="1"/>
-    <col min="29" max="29" width="6.33203125" customWidth="1"/>
+    <col min="20" max="20" width="5.85546875" customWidth="1"/>
+    <col min="21" max="21" width="11.42578125" customWidth="1"/>
+    <col min="22" max="22" width="10.85546875" customWidth="1"/>
+    <col min="23" max="23" width="9.85546875" customWidth="1"/>
+    <col min="24" max="24" width="13.7109375" customWidth="1"/>
+    <col min="25" max="25" width="11.140625" customWidth="1"/>
+    <col min="26" max="26" width="8.7109375" customWidth="1"/>
+    <col min="27" max="28" width="5.85546875" customWidth="1"/>
+    <col min="29" max="29" width="6.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -915,7 +925,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:29" x14ac:dyDescent="0.25">
       <c r="E2" s="4" t="s">
         <v>5</v>
       </c>
@@ -974,13 +984,14 @@
       </c>
       <c r="AC2" s="2"/>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="B3" t="s">
-        <v>39</v>
-      </c>
+        <v>126</v>
+      </c>
+      <c r="D3" s="5"/>
       <c r="E3">
         <v>0.4</v>
       </c>
@@ -1027,13 +1038,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>222</v>
       </c>
       <c r="B4" t="s">
-        <v>40</v>
-      </c>
+        <v>127</v>
+      </c>
+      <c r="D4" s="5"/>
       <c r="E4">
         <v>0.4</v>
       </c>
@@ -1080,13 +1092,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>333</v>
       </c>
       <c r="B5" t="s">
-        <v>41</v>
-      </c>
+        <v>128</v>
+      </c>
+      <c r="D5" s="5"/>
       <c r="E5">
         <v>0.4</v>
       </c>
@@ -1133,13 +1146,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>444</v>
       </c>
       <c r="B6" t="s">
-        <v>42</v>
-      </c>
+        <v>129</v>
+      </c>
+      <c r="D6" s="5"/>
       <c r="E6">
         <v>0.4</v>
       </c>
@@ -1187,6 +1201,7 @@
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1199,115 +1214,114 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.88671875" customWidth="1"/>
-    <col min="2" max="2" width="12.6640625" customWidth="1"/>
-    <col min="3" max="3" width="14.77734375" customWidth="1"/>
-    <col min="4" max="4" width="9.21875" customWidth="1"/>
-    <col min="5" max="5" width="11.109375" customWidth="1"/>
-    <col min="6" max="6" width="12.6640625" customWidth="1"/>
-    <col min="7" max="7" width="7.33203125" customWidth="1"/>
-    <col min="8" max="8" width="5.88671875" customWidth="1"/>
-    <col min="9" max="9" width="16.44140625" customWidth="1"/>
-    <col min="10" max="10" width="5.88671875" customWidth="1"/>
-    <col min="11" max="11" width="6.77734375" customWidth="1"/>
-    <col min="12" max="12" width="6.6640625" customWidth="1"/>
-    <col min="13" max="13" width="5.88671875" customWidth="1"/>
-    <col min="14" max="15" width="9.21875" customWidth="1"/>
-    <col min="16" max="16" width="6.88671875" customWidth="1"/>
-    <col min="17" max="18" width="9.21875" customWidth="1"/>
-    <col min="19" max="19" width="6.88671875" customWidth="1"/>
-    <col min="20" max="20" width="6.5546875" customWidth="1"/>
-    <col min="21" max="21" width="5.88671875" customWidth="1"/>
-    <col min="22" max="22" width="7.77734375" customWidth="1"/>
+    <col min="1" max="1" width="14.85546875" customWidth="1"/>
+    <col min="2" max="2" width="12.7109375" customWidth="1"/>
+    <col min="3" max="3" width="14.7109375" customWidth="1"/>
+    <col min="4" max="4" width="9.28515625" customWidth="1"/>
+    <col min="5" max="5" width="11.140625" customWidth="1"/>
+    <col min="6" max="6" width="12.7109375" customWidth="1"/>
+    <col min="7" max="7" width="7.28515625" customWidth="1"/>
+    <col min="8" max="8" width="5.85546875" customWidth="1"/>
+    <col min="9" max="9" width="16.42578125" customWidth="1"/>
+    <col min="10" max="10" width="5.85546875" customWidth="1"/>
+    <col min="11" max="12" width="6.7109375" customWidth="1"/>
+    <col min="13" max="13" width="5.85546875" customWidth="1"/>
+    <col min="14" max="15" width="9.28515625" customWidth="1"/>
+    <col min="16" max="16" width="6.85546875" customWidth="1"/>
+    <col min="17" max="18" width="9.28515625" customWidth="1"/>
+    <col min="19" max="19" width="6.85546875" customWidth="1"/>
+    <col min="20" max="20" width="6.5703125" customWidth="1"/>
+    <col min="21" max="21" width="5.85546875" customWidth="1"/>
+    <col min="22" max="22" width="7.7109375" customWidth="1"/>
     <col min="23" max="23" width="11" customWidth="1"/>
-    <col min="24" max="24" width="14.21875" customWidth="1"/>
+    <col min="24" max="24" width="14.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="F1" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="G1" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>49</v>
       </c>
       <c r="H1" s="3" t="s">
         <v>22</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="L1" s="3" t="s">
         <v>4</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>55</v>
+        <v>52</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="S1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="V1" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>69</v>
-      </c>
       <c r="X1" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
       <c r="F2" s="2"/>
       <c r="G2" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>23</v>
@@ -1315,51 +1329,51 @@
       <c r="I2" s="4"/>
       <c r="J2" s="4"/>
       <c r="K2" s="4" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="L2" s="4" t="s">
         <v>5</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>56</v>
+        <v>53</v>
       </c>
       <c r="N2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="O2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="P2" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="O2" s="4" t="s">
+      <c r="Q2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="S2" s="4" t="s">
         <v>58</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="Q2" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>58</v>
-      </c>
-      <c r="S2" s="4" t="s">
-        <v>61</v>
       </c>
       <c r="T2" s="4" t="s">
         <v>25</v>
       </c>
       <c r="U2" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="V2" s="4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="W2" s="4" t="s">
         <v>30</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4</v>
+        <v>444</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -1368,7 +1382,7 @@
         <v>1</v>
       </c>
       <c r="F3" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G3">
         <v>100</v>
@@ -1422,9 +1436,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5</v>
+        <v>555</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -1433,7 +1447,7 @@
         <v>1</v>
       </c>
       <c r="F4" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G4">
         <v>100</v>
@@ -1487,9 +1501,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>6</v>
+        <v>666</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -1498,7 +1512,7 @@
         <v>1</v>
       </c>
       <c r="F5" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="G5">
         <v>100</v>
@@ -1565,43 +1579,43 @@
       <pane xSplit="3" ySplit="2" topLeftCell="D3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight"/>
+      <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.77734375" customWidth="1"/>
-    <col min="2" max="2" width="6.5546875" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.5546875" customWidth="1"/>
-    <col min="5" max="5" width="12.33203125" customWidth="1"/>
-    <col min="6" max="6" width="8.5546875" customWidth="1"/>
-    <col min="7" max="7" width="11.21875" customWidth="1"/>
-    <col min="8" max="8" width="18.5546875" customWidth="1"/>
-    <col min="9" max="9" width="11.88671875" customWidth="1"/>
-    <col min="10" max="10" width="9.6640625" customWidth="1"/>
-    <col min="11" max="11" width="5.88671875" customWidth="1"/>
-    <col min="12" max="12" width="8.44140625" customWidth="1"/>
-    <col min="13" max="13" width="15.88671875" customWidth="1"/>
-    <col min="14" max="14" width="17.88671875" customWidth="1"/>
-    <col min="15" max="15" width="16.21875" customWidth="1"/>
-    <col min="16" max="16" width="24.21875" customWidth="1"/>
-    <col min="17" max="17" width="22.88671875" customWidth="1"/>
-    <col min="18" max="18" width="23.5546875" customWidth="1"/>
-    <col min="19" max="19" width="7.33203125" customWidth="1"/>
-    <col min="20" max="20" width="6.33203125" customWidth="1"/>
-    <col min="21" max="21" width="6.5546875" customWidth="1"/>
-    <col min="22" max="22" width="9.6640625" customWidth="1"/>
-    <col min="23" max="24" width="7.33203125" customWidth="1"/>
-    <col min="25" max="26" width="9.6640625" customWidth="1"/>
-    <col min="27" max="27" width="6.109375" customWidth="1"/>
-    <col min="28" max="28" width="5.88671875" customWidth="1"/>
+    <col min="1" max="1" width="8.7109375" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.5703125" customWidth="1"/>
+    <col min="5" max="5" width="12.28515625" customWidth="1"/>
+    <col min="6" max="6" width="8.5703125" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" customWidth="1"/>
+    <col min="8" max="8" width="18.5703125" customWidth="1"/>
+    <col min="9" max="9" width="11.85546875" customWidth="1"/>
+    <col min="10" max="10" width="9.7109375" customWidth="1"/>
+    <col min="11" max="11" width="5.85546875" customWidth="1"/>
+    <col min="12" max="12" width="8.42578125" customWidth="1"/>
+    <col min="13" max="13" width="15.85546875" customWidth="1"/>
+    <col min="14" max="14" width="17.85546875" customWidth="1"/>
+    <col min="15" max="15" width="16.28515625" customWidth="1"/>
+    <col min="16" max="16" width="24.28515625" customWidth="1"/>
+    <col min="17" max="17" width="22.85546875" customWidth="1"/>
+    <col min="18" max="18" width="23.5703125" customWidth="1"/>
+    <col min="19" max="19" width="7.28515625" customWidth="1"/>
+    <col min="20" max="20" width="6.28515625" customWidth="1"/>
+    <col min="21" max="21" width="6.5703125" customWidth="1"/>
+    <col min="22" max="22" width="9.7109375" customWidth="1"/>
+    <col min="23" max="24" width="7.28515625" customWidth="1"/>
+    <col min="25" max="26" width="9.7109375" customWidth="1"/>
+    <col min="27" max="27" width="6.140625" customWidth="1"/>
+    <col min="28" max="28" width="5.85546875" customWidth="1"/>
     <col min="29" max="29" width="13" customWidth="1"/>
-    <col min="30" max="30" width="7.5546875" customWidth="1"/>
-    <col min="31" max="31" width="22.88671875" customWidth="1"/>
+    <col min="30" max="30" width="7.5703125" customWidth="1"/>
+    <col min="31" max="31" width="22.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -1612,34 +1626,34 @@
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="L1" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>79</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>80</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="N1" s="3" t="s">
         <v>12</v>
@@ -1657,48 +1671,48 @@
         <v>18</v>
       </c>
       <c r="S1" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="T1" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="AA1" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="AB1" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="AC1" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="U1" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="V1" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="W1" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="X1" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="Y1" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="AA1" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="AB1" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="AC1" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="AD1" s="3" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="AE1" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="N2" s="4" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>15</v>
@@ -1713,7 +1727,7 @@
         <v>15</v>
       </c>
       <c r="S2" s="4" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="T2" s="4" t="s">
         <v>23</v>
@@ -1728,7 +1742,7 @@
         <v>36</v>
       </c>
       <c r="X2" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="Y2" s="4" t="s">
         <v>36</v>
@@ -1737,10 +1751,10 @@
         <v>36</v>
       </c>
       <c r="AA2" s="4" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="AB2" s="4" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="AC2" s="4"/>
       <c r="AD2" s="4"/>
@@ -1748,27 +1762,27 @@
         <v>13</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>4</v>
+        <v>444</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="E3" t="s">
-        <v>39</v>
+        <v>126</v>
       </c>
       <c r="H3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I3">
-        <v>2</v>
+        <v>222</v>
       </c>
       <c r="J3" t="s">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="M3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N3">
         <v>0</v>
@@ -1825,27 +1839,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>5</v>
+        <v>555</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>222</v>
       </c>
       <c r="E4" t="s">
-        <v>40</v>
+        <v>127</v>
       </c>
       <c r="H4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I4">
-        <v>3</v>
+        <v>333</v>
       </c>
       <c r="J4" t="s">
-        <v>41</v>
+        <v>128</v>
       </c>
       <c r="M4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N4">
         <v>0</v>
@@ -1902,27 +1916,27 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>6</v>
+        <v>666</v>
       </c>
       <c r="D5">
-        <v>2</v>
+        <v>333</v>
       </c>
       <c r="E5" t="s">
-        <v>40</v>
+        <v>128</v>
       </c>
       <c r="H5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I5">
-        <v>4</v>
+        <v>444</v>
       </c>
       <c r="J5" t="s">
-        <v>42</v>
+        <v>129</v>
       </c>
       <c r="M5" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="N5">
         <v>0</v>
@@ -1995,34 +2009,34 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="2" max="2" width="11.88671875" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" customWidth="1"/>
-    <col min="11" max="11" width="24.21875" customWidth="1"/>
-    <col min="12" max="12" width="22.88671875" customWidth="1"/>
-    <col min="13" max="13" width="23.5546875" customWidth="1"/>
-    <col min="14" max="14" width="5.88671875" customWidth="1"/>
-    <col min="15" max="15" width="6.33203125" customWidth="1"/>
-    <col min="16" max="16" width="8.44140625" customWidth="1"/>
-    <col min="17" max="17" width="7.77734375" customWidth="1"/>
-    <col min="18" max="18" width="8.21875" customWidth="1"/>
-    <col min="19" max="19" width="5.88671875" customWidth="1"/>
-    <col min="20" max="20" width="6.33203125" customWidth="1"/>
-    <col min="21" max="21" width="7.77734375" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="11" max="11" width="24.28515625" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" customWidth="1"/>
+    <col min="14" max="14" width="5.85546875" customWidth="1"/>
+    <col min="15" max="15" width="6.28515625" customWidth="1"/>
+    <col min="16" max="16" width="8.42578125" customWidth="1"/>
+    <col min="17" max="17" width="7.7109375" customWidth="1"/>
+    <col min="18" max="18" width="8.28515625" customWidth="1"/>
+    <col min="19" max="19" width="5.85546875" customWidth="1"/>
+    <col min="20" max="20" width="6.28515625" customWidth="1"/>
+    <col min="21" max="21" width="7.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2031,19 +2045,19 @@
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>12</v>
@@ -2061,31 +2075,31 @@
         <v>18</v>
       </c>
       <c r="N1" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="Q1" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="R1" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="U1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="S1" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>106</v>
-      </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
       <c r="H2" s="2"/>
       <c r="I2" s="4" t="s">
         <v>13</v>
@@ -2103,39 +2117,39 @@
         <v>15</v>
       </c>
       <c r="N2" s="4" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="O2" s="4" t="s">
         <v>34</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="Q2" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="R2" s="4" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="S2" s="4"/>
       <c r="T2" s="4"/>
       <c r="U2" s="2"/>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>111</v>
       </c>
       <c r="E3" t="s">
         <v>39</v>
       </c>
       <c r="H3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2174,7 +2188,7 @@
         <v>3</v>
       </c>
       <c r="U3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>
@@ -2193,38 +2207,38 @@
       <selection pane="bottomRight"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="12.109375" customWidth="1"/>
-    <col min="2" max="2" width="6.5546875" customWidth="1"/>
-    <col min="3" max="3" width="5.88671875" customWidth="1"/>
-    <col min="4" max="4" width="14.77734375" customWidth="1"/>
-    <col min="5" max="5" width="12.5546875" customWidth="1"/>
-    <col min="6" max="6" width="8.77734375" customWidth="1"/>
-    <col min="7" max="7" width="7.44140625" customWidth="1"/>
-    <col min="8" max="8" width="12.77734375" customWidth="1"/>
-    <col min="9" max="9" width="17.88671875" customWidth="1"/>
-    <col min="10" max="10" width="16.21875" customWidth="1"/>
-    <col min="11" max="11" width="24.21875" customWidth="1"/>
-    <col min="12" max="12" width="22.88671875" customWidth="1"/>
-    <col min="13" max="13" width="23.5546875" customWidth="1"/>
-    <col min="14" max="14" width="14.33203125" customWidth="1"/>
-    <col min="15" max="16" width="5.88671875" customWidth="1"/>
-    <col min="17" max="17" width="16.109375" customWidth="1"/>
-    <col min="18" max="18" width="8.21875" customWidth="1"/>
-    <col min="19" max="19" width="7.77734375" customWidth="1"/>
-    <col min="20" max="20" width="12.44140625" customWidth="1"/>
-    <col min="21" max="22" width="23.33203125" customWidth="1"/>
-    <col min="23" max="23" width="9.5546875" customWidth="1"/>
+    <col min="1" max="1" width="12.140625" customWidth="1"/>
+    <col min="2" max="2" width="6.5703125" customWidth="1"/>
+    <col min="3" max="3" width="5.85546875" customWidth="1"/>
+    <col min="4" max="4" width="14.7109375" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" customWidth="1"/>
+    <col min="6" max="6" width="8.7109375" customWidth="1"/>
+    <col min="7" max="7" width="7.42578125" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="17.85546875" customWidth="1"/>
+    <col min="10" max="10" width="16.28515625" customWidth="1"/>
+    <col min="11" max="11" width="24.28515625" customWidth="1"/>
+    <col min="12" max="12" width="22.85546875" customWidth="1"/>
+    <col min="13" max="13" width="23.5703125" customWidth="1"/>
+    <col min="14" max="14" width="14.28515625" customWidth="1"/>
+    <col min="15" max="16" width="5.85546875" customWidth="1"/>
+    <col min="17" max="17" width="16.140625" customWidth="1"/>
+    <col min="18" max="18" width="8.28515625" customWidth="1"/>
+    <col min="19" max="19" width="7.7109375" customWidth="1"/>
+    <col min="20" max="20" width="12.42578125" customWidth="1"/>
+    <col min="21" max="22" width="23.28515625" customWidth="1"/>
+    <col min="23" max="23" width="9.5703125" customWidth="1"/>
     <col min="24" max="24" width="18" customWidth="1"/>
-    <col min="25" max="25" width="22.21875" customWidth="1"/>
-    <col min="26" max="26" width="18.109375" customWidth="1"/>
-    <col min="27" max="27" width="15.21875" customWidth="1"/>
+    <col min="25" max="25" width="22.28515625" customWidth="1"/>
+    <col min="26" max="26" width="18.140625" customWidth="1"/>
+    <col min="27" max="27" width="15.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>1</v>
@@ -2233,19 +2247,19 @@
         <v>3</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>93</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>94</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>96</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>12</v>
@@ -2263,49 +2277,49 @@
         <v>18</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="P1" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="O1" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="R1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="S1" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="S1" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="T1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="X1" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="Y1" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="Z1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="X1" s="3" t="s">
+      <c r="AA1" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="Y1" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="Z1" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="AA1" s="1" t="s">
-        <v>123</v>
-      </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="H2" s="2"/>
       <c r="I2" s="4" t="s">
         <v>13</v>
@@ -2324,10 +2338,10 @@
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="4" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="P2" s="4" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="Q2" s="2"/>
       <c r="R2" s="2"/>
@@ -2341,18 +2355,18 @@
       <c r="Z2" s="4"/>
       <c r="AA2" s="2"/>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
       <c r="D3">
-        <v>3</v>
+        <v>333</v>
       </c>
       <c r="E3" t="s">
-        <v>41</v>
+        <v>128</v>
       </c>
       <c r="H3" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I3">
         <v>0</v>
@@ -2376,13 +2390,13 @@
         <v>0</v>
       </c>
       <c r="Q3" t="s">
-        <v>125</v>
+        <v>122</v>
       </c>
       <c r="R3" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="S3" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="X3">
         <v>0</v>
@@ -2394,18 +2408,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
       <c r="D4">
-        <v>4</v>
+        <v>444</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>129</v>
       </c>
       <c r="H4" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="I4">
         <v>0</v>
@@ -2429,22 +2443,22 @@
         <v>0.01</v>
       </c>
       <c r="Q4" t="s">
+        <v>122</v>
+      </c>
+      <c r="R4" t="s">
+        <v>121</v>
+      </c>
+      <c r="S4" t="s">
+        <v>105</v>
+      </c>
+      <c r="T4" t="s">
+        <v>123</v>
+      </c>
+      <c r="U4" t="s">
+        <v>124</v>
+      </c>
+      <c r="V4" t="s">
         <v>125</v>
-      </c>
-      <c r="R4" t="s">
-        <v>124</v>
-      </c>
-      <c r="S4" t="s">
-        <v>108</v>
-      </c>
-      <c r="T4" t="s">
-        <v>126</v>
-      </c>
-      <c r="U4" t="s">
-        <v>127</v>
-      </c>
-      <c r="V4" t="s">
-        <v>128</v>
       </c>
       <c r="X4">
         <v>0</v>

</xml_diff>